<commit_message>
updated steps,feature,pageobj for array,queue
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimre\eclipse-workspace\DSAlgoBDD_ClubNinjas\clubNinjas-BDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8B7E80-6FBF-4BED-B9C6-B7907F57D583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADCE862-317A-4206-B652-EA4A6D4D0F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
     <sheet name="Valid_Login" sheetId="3" r:id="rId2"/>
     <sheet name="Login" sheetId="1" r:id="rId3"/>
-    <sheet name="ArrayTryCode" sheetId="4" r:id="rId4"/>
+    <sheet name="TryCode" sheetId="4" r:id="rId4"/>
     <sheet name="PracticeQns" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -335,7 +335,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -378,6 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2067,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6805FF-85F8-4503-AEFF-417C4DCED9F7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2124,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C156544-10E3-4CC6-B021-D85ABA7773B9}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2213,7 +2214,7 @@
       <c r="A8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="20">
         <v>3</v>
       </c>
       <c r="C8" t="s">
@@ -2235,7 +2236,7 @@
       <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="20">
         <v>2</v>
       </c>
       <c r="C10" t="s">

</xml_diff>

<commit_message>
Added code for graph feature and updated other testSteps
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skurr\eclipse-workspace\ClubNinjas-dsAlgoBDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC68FB1E-4E6C-41BD-AB5C-1595D9FCCD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E85AA-EB45-466F-9582-E196C2657BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
     <sheet name="Valid_Login" sheetId="3" r:id="rId2"/>
     <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Graph" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>UserName</t>
   </si>
@@ -50,22 +51,10 @@
     <t>Testbuster@123</t>
   </si>
   <si>
-    <t>Error on confirm password feilds. Pass</t>
-  </si>
-  <si>
     <t>One password left blank.Error</t>
   </si>
   <si>
-    <t>Error on password feild. Pass</t>
-  </si>
-  <si>
-    <t>Defect. Password feilds are accpeting commenly used words</t>
-  </si>
-  <si>
     <t>Commonly used</t>
-  </si>
-  <si>
-    <t>Defect. Password feilds are accepting entire numeric data.</t>
   </si>
   <si>
     <t>Can't be completely numeric. Error</t>
@@ -81,18 +70,12 @@
     <t>test098</t>
   </si>
   <si>
-    <t>Error in Username feild which is valid</t>
-  </si>
-  <si>
     <t>Valid Passwords</t>
   </si>
   <si>
     <t>Test_987</t>
   </si>
   <si>
-    <t>Defect. Shows Password Mismatch error when user enters valid password in both feilds. If no password is entered or passwords is entered then it shows password feild is required but no error is shown that user username is invalid.</t>
-  </si>
-  <si>
     <t>Invalid Username error</t>
   </si>
   <si>
@@ -136,13 +119,85 @@
   </si>
   <si>
     <t>clubNinjas-Sdet207&amp;%^()</t>
+  </si>
+  <si>
+    <t>Defect. Password fields are accepting entire numeric data.</t>
+  </si>
+  <si>
+    <t>Defect. Password fields are accpeting commenly used words</t>
+  </si>
+  <si>
+    <t>Error on password field. Pass</t>
+  </si>
+  <si>
+    <t>Error on confirm password fields. Pass</t>
+  </si>
+  <si>
+    <t>Error in Username field which is valid</t>
+  </si>
+  <si>
+    <t>Defect. Shows Password Mismatch error when user enters valid password in both field. If no password is entered or passwords is entered then it shows password field is required but no error is shown that user username is invalid.</t>
+  </si>
+  <si>
+    <t>Defect. Shows Password Mismatch error when user enters valid password in both fields. If no password is entered or passwords is entered then it shows password feild is required but no error is shown that user username is invalid.</t>
+  </si>
+  <si>
+    <t>pythoncode</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>print "hello"</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>A23df</t>
+  </si>
+  <si>
+    <t>NameError: name 'A23df' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>alphanumeric check</t>
+  </si>
+  <si>
+    <t>number check</t>
+  </si>
+  <si>
+    <t>$%%^$^</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad token T_OP on line 1</t>
+  </si>
+  <si>
+    <t>special charecters check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
+  <si>
+    <t>Error:input some data</t>
+  </si>
+  <si>
+    <t>blank space check</t>
+  </si>
+  <si>
+    <t>print "hello</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>syntax check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +240,23 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -217,13 +289,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -251,6 +338,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -539,7 +633,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -555,27 +649,27 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
@@ -586,7 +680,7 @@
         <v>207207208</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="5"/>
@@ -594,12 +688,12 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -607,7 +701,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -619,7 +713,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -628,10 +722,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -639,7 +733,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -648,10 +742,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -665,10 +759,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
@@ -677,16 +771,16 @@
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
@@ -694,26 +788,26 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9">
         <v>987654321</v>
@@ -722,10 +816,10 @@
         <v>987654321</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
@@ -733,7 +827,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1</v>
@@ -742,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
@@ -753,16 +847,16 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -770,17 +864,17 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -788,7 +882,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>5</v>
@@ -1828,7 +1922,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1839,10 +1933,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1865,7 +1959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1903,13 +1997,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1934,4 +2028,94 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F35F7A1-F140-4775-834A-27596D852A38}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="19">
+        <v>123434</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved the excel data conflict
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skurr\eclipse-workspace\ClubNinjas-dsAlgoBDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E85AA-EB45-466F-9582-E196C2657BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B604879-F2A7-4068-984C-ADEE3288ED59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
-    <sheet name="Valid_Login" sheetId="3" r:id="rId2"/>
-    <sheet name="Login" sheetId="1" r:id="rId3"/>
-    <sheet name="Graph" sheetId="4" r:id="rId4"/>
+    <sheet name="Graph" sheetId="6" r:id="rId2"/>
+    <sheet name="Valid_Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="TryCode" sheetId="4" r:id="rId5"/>
+    <sheet name="PracticeQns" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>UserName</t>
   </si>
@@ -51,10 +53,22 @@
     <t>Testbuster@123</t>
   </si>
   <si>
+    <t>Error on confirm password feilds. Pass</t>
+  </si>
+  <si>
     <t>One password left blank.Error</t>
   </si>
   <si>
+    <t>Error on password feild. Pass</t>
+  </si>
+  <si>
+    <t>Defect. Password feilds are accpeting commenly used words</t>
+  </si>
+  <si>
     <t>Commonly used</t>
+  </si>
+  <si>
+    <t>Defect. Password feilds are accepting entire numeric data.</t>
   </si>
   <si>
     <t>Can't be completely numeric. Error</t>
@@ -70,12 +84,18 @@
     <t>test098</t>
   </si>
   <si>
+    <t>Error in Username feild which is valid</t>
+  </si>
+  <si>
     <t>Valid Passwords</t>
   </si>
   <si>
     <t>Test_987</t>
   </si>
   <si>
+    <t>Defect. Shows Password Mismatch error when user enters valid password in both feilds. If no password is entered or passwords is entered then it shows password feild is required but no error is shown that user username is invalid.</t>
+  </si>
+  <si>
     <t>Invalid Username error</t>
   </si>
   <si>
@@ -121,25 +141,93 @@
     <t>clubNinjas-Sdet207&amp;%^()</t>
   </si>
   <si>
-    <t>Defect. Password fields are accepting entire numeric data.</t>
-  </si>
-  <si>
-    <t>Defect. Password fields are accpeting commenly used words</t>
-  </si>
-  <si>
-    <t>Error on password field. Pass</t>
-  </si>
-  <si>
-    <t>Error on confirm password fields. Pass</t>
-  </si>
-  <si>
-    <t>Error in Username field which is valid</t>
-  </si>
-  <si>
-    <t>Defect. Shows Password Mismatch error when user enters valid password in both field. If no password is entered or passwords is entered then it shows password field is required but no error is shown that user username is invalid.</t>
-  </si>
-  <si>
-    <t>Defect. Shows Password Mismatch error when user enters valid password in both fields. If no password is entered or passwords is entered then it shows password feild is required but no error is shown that user username is invalid.</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>print("Hello, World!"</t>
+  </si>
+  <si>
+    <t>SyntaxError</t>
+  </si>
+  <si>
+    <t>prin("Hello, World!")</t>
+  </si>
+  <si>
+    <t>NameError</t>
+  </si>
+  <si>
+    <t>print("Hello, World!")</t>
+  </si>
+  <si>
+    <t>Hello, World!</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>SUBMIT</t>
+  </si>
+  <si>
+    <t>def search(input_list, num): 
+    if (num in input_list):
+        print("Element Found")
+    else:
+        print("Not Found")
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+	count = 0
+	result = 0
+	for i in range(0, len(nums)):
+		if (nums[i] == 0):
+			count = 0
+		else:
+			count+= 1
+			result = max(result, count)
+	print(result)
+findMaxConsecutiveOnes([1,1,0,1,1,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+	c=0
+	for i in nums:
+		j=str(i)
+		x=len(j)
+		if x%2==0:
+			c=c+1
+	print(c)
+	return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+	squares_list = []
+	for i in range(0, len(nums)):
+		square = nums[i] * nums[i];
+		squares_list.append(square)
+	sorted_squares_list = sorted(squares_list)
+	print sorted_squares_list;
+	return sorted_squares_list;
+sortedSquares([-4,-1,0,3,10])</t>
+  </si>
+  <si>
+    <t>[0, 1, 9, 16, 100]</t>
   </si>
   <si>
     <t>pythoncode</t>
@@ -197,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +333,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -258,12 +361,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -310,7 +419,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -338,9 +447,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -633,7 +758,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -649,27 +774,27 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
@@ -680,7 +805,7 @@
         <v>207207208</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="5"/>
@@ -688,12 +813,12 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -701,7 +826,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -713,7 +838,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -722,10 +847,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -733,7 +858,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -742,10 +867,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -759,10 +884,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
@@ -771,16 +896,16 @@
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
@@ -788,26 +913,26 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B11" s="9">
         <v>987654321</v>
@@ -816,10 +941,10 @@
         <v>987654321</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
@@ -827,7 +952,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1</v>
@@ -836,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
@@ -847,16 +972,16 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -864,17 +989,17 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -882,7 +1007,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>5</v>
@@ -1918,11 +2043,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36287EC-5C35-4A53-A766-4648041612D3}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>123434</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19390E6-AB14-4B31-A0B5-2F88190D0871}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1933,10 +2148,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1955,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1997,13 +2212,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -2030,89 +2245,216 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F35F7A1-F140-4775-834A-27596D852A38}">
-  <dimension ref="A1:C7"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6805FF-85F8-4503-AEFF-417C4DCED9F7}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C156544-10E3-4CC6-B021-D85ABA7773B9}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.08984375" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
-        <v>123434</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B8" s="20">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="B10" s="20">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>